<commit_message>
Implemented load / save
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dokumente\!dhbw\6. semester\Flowchart-RealtimeSystems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9944C8A-13CC-49BF-A5D8-AE0B3E9021E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F937E209-18C9-4523-A097-D4C6E175EB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-60" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>INPUTS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>PRIORITY</t>
   </si>
   <si>
-    <t>OUTPUTS</t>
-  </si>
-  <si>
     <t>TASK</t>
   </si>
   <si>
-    <t>ACTIVITY + DURATION</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>POSX</t>
+  </si>
+  <si>
+    <t>POSY</t>
+  </si>
+  <si>
+    <t>ACTIVITY</t>
+  </si>
+  <si>
+    <t>CYCLES</t>
+  </si>
+  <si>
+    <t>CON_NAME</t>
+  </si>
+  <si>
+    <t>START</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>r3</t>
+  </si>
+  <si>
+    <t>r4</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>r5</t>
   </si>
 </sst>
 </file>
@@ -75,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -357,34 +403,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K1" sqref="K1:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="3" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1">
+        <v>150</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <v>300</v>
+      </c>
+      <c r="F4" s="1">
+        <v>50</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>